<commit_message>
MS1 Part2 B second submission
</commit_message>
<xml_diff>
--- a/hymm-limitless-coders-MS1-P2-B.xlsx
+++ b/hymm-limitless-coders-MS1-P2-B.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -676,33 +676,6 @@
     <t>Messaging Scalability</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="17"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The notification service shall support sending alerts to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color indexed="17"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>up to 10,000 students concurrently</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color indexed="17"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> without performance degradation.</t>
-    </r>
-  </si>
-  <si>
     <t>The number of notifications successfully sent per second to be &gt;2000 notifications per second</t>
   </si>
   <si>
@@ -832,12 +805,15 @@
       <t>https://chatgpt.com/share/67f6cd05-13d4-8013-895f-e420a8368d90     (For non-functional requirements)</t>
     </r>
   </si>
+  <si>
+    <t>The notification service shall support sending alerts to up to 10,000 students concurrently without performance degradation.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -895,22 +871,11 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="17"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="17"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
@@ -923,8 +888,14 @@
       <color indexed="17"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,18 +928,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="20"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1126,26 +1091,6 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
       <right style="thin">
         <color indexed="12"/>
       </right>
@@ -1174,66 +1119,6 @@
       </top>
       <bottom style="thin">
         <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="19"/>
-      </right>
-      <top style="medium">
-        <color indexed="19"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="19"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1449,11 +1334,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="19"/>
+      </right>
+      <top style="medium">
+        <color indexed="19"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="19"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1478,73 +1470,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1579,61 +1527,97 @@
     <xf numFmtId="49" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2799,20 +2783,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B3" s="45" t="s">
+    <row r="3" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-    </row>
-    <row r="7" spans="2:4" ht="18">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -2823,14 +2807,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15">
+    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15">
+    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -2839,14 +2823,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15">
+    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15">
+    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -2855,14 +2839,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15">
+    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15">
+    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -2871,20 +2855,20 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15">
+    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15">
+    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2907,7 +2891,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="5" customWidth="1"/>
@@ -2916,46 +2900,46 @@
     <col min="7" max="16384" width="12.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="54.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
@@ -2970,7 +2954,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -2985,7 +2969,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
@@ -3000,7 +2984,7 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -3015,7 +2999,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
@@ -3030,7 +3014,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -3061,1132 +3045,1132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="13" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="13" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="13" customWidth="1"/>
     <col min="5" max="5" width="128.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="85.42578125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" style="66" customWidth="1"/>
+    <col min="6" max="6" width="85.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="48" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="13" customWidth="1"/>
     <col min="9" max="16384" width="12.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="67" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" thickTop="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64" t="s">
+    <row r="2" spans="1:7" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="75"/>
-    </row>
-    <row r="3" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A3" s="69" t="s">
+      <c r="G2" s="59"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="55">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="71">
+      <c r="B4" s="55">
         <v>1</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="55">
         <v>2</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="72"/>
-    </row>
-    <row r="5" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A5" s="70" t="s">
+      <c r="G4" s="56"/>
+    </row>
+    <row r="5" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="71">
+      <c r="B5" s="55">
         <v>1</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="55">
         <v>3</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="72"/>
-    </row>
-    <row r="6" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A6" s="70" t="s">
+      <c r="G5" s="56"/>
+    </row>
+    <row r="6" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="55">
         <v>1</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="55">
         <v>4</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="69" t="s">
+      <c r="G6" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A7" s="70" t="s">
+    <row r="7" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="55">
         <v>2</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="55">
         <v>5</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="72"/>
-    </row>
-    <row r="8" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A8" s="73" t="s">
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="71">
+      <c r="B8" s="55">
         <v>5</v>
       </c>
-      <c r="C8" s="71">
+      <c r="C8" s="55">
         <v>6</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="70" t="s">
+      <c r="F8" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="72"/>
-    </row>
-    <row r="9" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A9" s="70" t="s">
+      <c r="G8" s="56"/>
+    </row>
+    <row r="9" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="71">
+      <c r="B9" s="55">
         <v>6</v>
       </c>
-      <c r="C9" s="71">
+      <c r="C9" s="55">
         <v>7</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A10" s="70" t="s">
+    <row r="10" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="71">
+      <c r="B10" s="55">
         <v>6</v>
       </c>
-      <c r="C10" s="71">
+      <c r="C10" s="55">
         <v>8</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="72"/>
-    </row>
-    <row r="11" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A11" s="70" t="s">
+      <c r="G10" s="56"/>
+    </row>
+    <row r="11" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="55">
         <v>6</v>
       </c>
-      <c r="C11" s="71">
+      <c r="C11" s="55">
         <v>9</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="72"/>
-    </row>
-    <row r="12" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A12" s="70" t="s">
+      <c r="G11" s="56"/>
+    </row>
+    <row r="12" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="71">
+      <c r="B12" s="55">
         <v>6</v>
       </c>
-      <c r="C12" s="71">
+      <c r="C12" s="55">
         <v>10</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="72"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A13" s="70" t="s">
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="55">
         <v>6</v>
       </c>
-      <c r="C13" s="71">
+      <c r="C13" s="55">
         <v>11</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="72"/>
-    </row>
-    <row r="14" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A14" s="70" t="s">
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="71">
+      <c r="B14" s="55">
         <v>3</v>
       </c>
-      <c r="C14" s="71">
+      <c r="C14" s="55">
         <v>12</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="70" t="s">
+      <c r="F14" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="72"/>
-    </row>
-    <row r="15" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A15" s="70" t="s">
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="71">
+      <c r="C15" s="55">
         <v>13</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="F15" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A16" s="68" t="s">
+    <row r="16" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="71">
+      <c r="B16" s="55">
         <v>1</v>
       </c>
-      <c r="C16" s="71">
+      <c r="C16" s="55">
         <v>14</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="70" t="s">
+      <c r="F16" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="72"/>
-    </row>
-    <row r="17" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A17" s="68" t="s">
+      <c r="G16" s="56"/>
+    </row>
+    <row r="17" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="55">
         <v>1</v>
       </c>
-      <c r="C17" s="71">
+      <c r="C17" s="55">
         <v>15</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="F17" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="72"/>
-    </row>
-    <row r="18" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A18" s="70" t="s">
+      <c r="G17" s="56"/>
+    </row>
+    <row r="18" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="71">
+      <c r="B18" s="55">
         <v>1</v>
       </c>
-      <c r="C18" s="71">
+      <c r="C18" s="55">
         <v>16</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="70" t="s">
+      <c r="E18" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="70" t="s">
+      <c r="F18" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="72"/>
-    </row>
-    <row r="19" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A19" s="68" t="s">
+      <c r="G18" s="56"/>
+    </row>
+    <row r="19" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="77">
+      <c r="B19" s="61">
         <v>16</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="61">
         <v>17</v>
       </c>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="70" t="s">
+      <c r="E19" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="70" t="s">
+      <c r="F19" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="72"/>
-    </row>
-    <row r="20" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A20" s="70" t="s">
+      <c r="G19" s="56"/>
+    </row>
+    <row r="20" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="71">
+      <c r="B20" s="55">
         <v>17</v>
       </c>
-      <c r="C20" s="77">
+      <c r="C20" s="61">
         <v>18</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="70" t="s">
+      <c r="E20" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F20" s="70" t="s">
+      <c r="F20" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="72"/>
-    </row>
-    <row r="21" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A21" s="68" t="s">
+      <c r="G20" s="56"/>
+    </row>
+    <row r="21" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="77">
+      <c r="B21" s="61">
         <v>16</v>
       </c>
-      <c r="C21" s="77">
+      <c r="C21" s="61">
         <v>19</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="72"/>
-    </row>
-    <row r="22" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A22" s="68" t="s">
+      <c r="G21" s="56"/>
+    </row>
+    <row r="22" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="77">
+      <c r="B22" s="61">
         <v>19</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="61">
         <v>20</v>
       </c>
-      <c r="D22" s="68" t="s">
+      <c r="D22" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="72"/>
-    </row>
-    <row r="23" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A23" s="70" t="s">
+      <c r="G22" s="56"/>
+    </row>
+    <row r="23" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="71">
+      <c r="B23" s="55">
         <v>20</v>
       </c>
-      <c r="C23" s="71">
+      <c r="C23" s="55">
         <v>21</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="70" t="s">
+      <c r="E23" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="70" t="s">
+      <c r="F23" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="72"/>
-    </row>
-    <row r="24" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A24" s="70" t="s">
+      <c r="G23" s="56"/>
+    </row>
+    <row r="24" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="71">
+      <c r="B24" s="55">
         <v>20</v>
       </c>
-      <c r="C24" s="71">
+      <c r="C24" s="55">
         <v>22</v>
       </c>
-      <c r="D24" s="68" t="s">
+      <c r="D24" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="70" t="s">
+      <c r="E24" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="70" t="s">
+      <c r="F24" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="72"/>
-    </row>
-    <row r="25" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A25" s="70" t="s">
+      <c r="G24" s="56"/>
+    </row>
+    <row r="25" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="71">
+      <c r="B25" s="55">
         <v>1</v>
       </c>
-      <c r="C25" s="71">
+      <c r="C25" s="55">
         <v>23</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="70" t="s">
+      <c r="F25" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="G25" s="72"/>
-    </row>
-    <row r="26" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A26" s="70" t="s">
+      <c r="G25" s="56"/>
+    </row>
+    <row r="26" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="71">
+      <c r="B26" s="55">
         <v>23</v>
       </c>
-      <c r="C26" s="71">
+      <c r="C26" s="55">
         <v>24</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D26" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F26" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="72"/>
-    </row>
-    <row r="27" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A27" s="70" t="s">
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="71">
+      <c r="B27" s="55">
         <v>24</v>
       </c>
-      <c r="C27" s="71">
+      <c r="C27" s="55">
         <v>25</v>
       </c>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E27" s="70" t="s">
+      <c r="E27" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="70" t="s">
+      <c r="F27" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="G27" s="72"/>
-    </row>
-    <row r="28" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A28" s="70" t="s">
+      <c r="G27" s="56"/>
+    </row>
+    <row r="28" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="71">
+      <c r="B28" s="55">
         <v>25</v>
       </c>
-      <c r="C28" s="71">
+      <c r="C28" s="55">
         <v>26</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="70" t="s">
+      <c r="E28" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="70" t="s">
+      <c r="F28" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="72"/>
-    </row>
-    <row r="29" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A29" s="70" t="s">
+      <c r="G28" s="56"/>
+    </row>
+    <row r="29" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="71">
+      <c r="B29" s="55">
         <v>26</v>
       </c>
-      <c r="C29" s="71">
+      <c r="C29" s="55">
         <v>27</v>
       </c>
-      <c r="D29" s="68" t="s">
+      <c r="D29" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="70" t="s">
+      <c r="F29" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="72"/>
-    </row>
-    <row r="30" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A30" s="70" t="s">
+      <c r="G29" s="56"/>
+    </row>
+    <row r="30" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="71">
+      <c r="B30" s="55">
         <v>27</v>
       </c>
-      <c r="C30" s="71">
+      <c r="C30" s="55">
         <v>28</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="70" t="s">
+      <c r="E30" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="70" t="s">
+      <c r="F30" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="72"/>
-    </row>
-    <row r="31" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A31" s="70" t="s">
+      <c r="G30" s="56"/>
+    </row>
+    <row r="31" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="71">
+      <c r="B31" s="55">
         <v>1</v>
       </c>
-      <c r="C31" s="71">
+      <c r="C31" s="55">
         <v>29</v>
       </c>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="70" t="s">
+      <c r="E31" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="70" t="s">
+      <c r="F31" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="G31" s="72"/>
-    </row>
-    <row r="32" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A32" s="70" t="s">
+      <c r="G31" s="56"/>
+    </row>
+    <row r="32" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="B32" s="71">
+      <c r="B32" s="55">
         <v>16</v>
       </c>
-      <c r="C32" s="71">
+      <c r="C32" s="55">
         <v>30</v>
       </c>
-      <c r="D32" s="68" t="s">
+      <c r="D32" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="70" t="s">
+      <c r="F32" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="G32" s="72"/>
-    </row>
-    <row r="33" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A33" s="70" t="s">
+      <c r="G32" s="56"/>
+    </row>
+    <row r="33" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="B33" s="71">
+      <c r="B33" s="55">
         <v>30</v>
       </c>
-      <c r="C33" s="71">
+      <c r="C33" s="55">
         <v>31</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="F33" s="70" t="s">
+      <c r="F33" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="G33" s="72"/>
-    </row>
-    <row r="34" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A34" s="70" t="s">
+      <c r="G33" s="56"/>
+    </row>
+    <row r="34" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="71">
+      <c r="B34" s="55">
         <v>29</v>
       </c>
-      <c r="C34" s="71">
+      <c r="C34" s="55">
         <v>32</v>
       </c>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="G34" s="73" t="s">
+      <c r="G34" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A35" s="70" t="s">
+    <row r="35" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="71">
+      <c r="B35" s="55">
         <v>29</v>
       </c>
-      <c r="C35" s="71">
+      <c r="C35" s="55">
         <v>33</v>
       </c>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="70" t="s">
+      <c r="E35" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="F35" s="70" t="s">
+      <c r="F35" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="G35" s="72"/>
-    </row>
-    <row r="36" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A36" s="70" t="s">
+      <c r="G35" s="56"/>
+    </row>
+    <row r="36" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="71">
+      <c r="B36" s="55">
         <v>29</v>
       </c>
-      <c r="C36" s="71">
+      <c r="C36" s="55">
         <v>34</v>
       </c>
-      <c r="D36" s="68" t="s">
+      <c r="D36" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="70" t="s">
+      <c r="E36" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="F36" s="70" t="s">
+      <c r="F36" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="73" t="s">
+      <c r="G36" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A37" s="70" t="s">
+    <row r="37" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="71">
+      <c r="B37" s="55">
         <v>29</v>
       </c>
-      <c r="C37" s="71">
+      <c r="C37" s="55">
         <v>35</v>
       </c>
-      <c r="D37" s="68" t="s">
+      <c r="D37" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="70" t="s">
+      <c r="E37" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="F37" s="70" t="s">
+      <c r="F37" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="G37" s="72"/>
-    </row>
-    <row r="38" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A38" s="70" t="s">
+      <c r="G37" s="56"/>
+    </row>
+    <row r="38" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="B38" s="71">
+      <c r="B38" s="55">
         <v>16</v>
       </c>
-      <c r="C38" s="71">
+      <c r="C38" s="55">
         <v>36</v>
       </c>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="70" t="s">
+      <c r="E38" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="F38" s="70" t="s">
+      <c r="F38" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="G38" s="72"/>
-    </row>
-    <row r="39" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A39" s="70" t="s">
+      <c r="G38" s="56"/>
+    </row>
+    <row r="39" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="71">
+      <c r="B39" s="55">
         <v>16</v>
       </c>
-      <c r="C39" s="71">
+      <c r="C39" s="55">
         <v>37</v>
       </c>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="70" t="s">
+      <c r="E39" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="70" t="s">
+      <c r="F39" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="G39" s="73" t="s">
+      <c r="G39" s="57" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A40" s="70" t="s">
+    <row r="40" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="71">
+      <c r="B40" s="55">
         <v>35</v>
       </c>
-      <c r="C40" s="71">
+      <c r="C40" s="55">
         <v>38</v>
       </c>
-      <c r="D40" s="68" t="s">
+      <c r="D40" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="70" t="s">
+      <c r="E40" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="F40" s="70" t="s">
+      <c r="F40" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="G40" s="72"/>
-    </row>
-    <row r="41" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A41" s="70" t="s">
+      <c r="G40" s="56"/>
+    </row>
+    <row r="41" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="B41" s="71">
+      <c r="B41" s="55">
         <v>15</v>
       </c>
-      <c r="C41" s="71">
+      <c r="C41" s="55">
         <v>39</v>
       </c>
-      <c r="D41" s="68" t="s">
+      <c r="D41" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="70" t="s">
+      <c r="E41" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="F41" s="70" t="s">
+      <c r="F41" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="G41" s="72"/>
-    </row>
-    <row r="42" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A42" s="70" t="s">
+      <c r="G41" s="56"/>
+    </row>
+    <row r="42" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="B42" s="71">
+      <c r="B42" s="55">
         <v>14</v>
       </c>
-      <c r="C42" s="71">
+      <c r="C42" s="55">
         <v>40</v>
       </c>
-      <c r="D42" s="68" t="s">
+      <c r="D42" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="70" t="s">
+      <c r="E42" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="G42" s="72"/>
-    </row>
-    <row r="43" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A43" s="70" t="s">
+      <c r="G42" s="56"/>
+    </row>
+    <row r="43" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="B43" s="71">
+      <c r="B43" s="55">
         <v>23</v>
       </c>
-      <c r="C43" s="71">
+      <c r="C43" s="55">
         <v>41</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="E43" s="70" t="s">
+      <c r="E43" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="70" t="s">
+      <c r="F43" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="G43" s="72"/>
-    </row>
-    <row r="44" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A44" s="70" t="s">
+      <c r="G43" s="56"/>
+    </row>
+    <row r="44" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="71">
+      <c r="B44" s="55">
         <v>41</v>
       </c>
-      <c r="C44" s="71">
+      <c r="C44" s="55">
         <v>42</v>
       </c>
-      <c r="D44" s="68" t="s">
+      <c r="D44" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="E44" s="70" t="s">
+      <c r="E44" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="F44" s="70" t="s">
+      <c r="F44" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="G44" s="72"/>
-    </row>
-    <row r="45" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A45" s="70" t="s">
+      <c r="G44" s="56"/>
+    </row>
+    <row r="45" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="B45" s="71">
+      <c r="B45" s="55">
         <v>41</v>
       </c>
-      <c r="C45" s="71">
+      <c r="C45" s="55">
         <v>43</v>
       </c>
-      <c r="D45" s="68" t="s">
+      <c r="D45" s="51" t="s">
         <v>168</v>
       </c>
-      <c r="E45" s="70" t="s">
+      <c r="E45" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="F45" s="70" t="s">
+      <c r="F45" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="G45" s="72"/>
-    </row>
-    <row r="46" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A46" s="70" t="s">
+      <c r="G45" s="56"/>
+    </row>
+    <row r="46" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="71">
+      <c r="B46" s="55">
         <v>42</v>
       </c>
-      <c r="C46" s="71">
+      <c r="C46" s="55">
         <v>44</v>
       </c>
-      <c r="D46" s="68" t="s">
+      <c r="D46" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="E46" s="70" t="s">
+      <c r="E46" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="F46" s="70" t="s">
+      <c r="F46" s="54" t="s">
         <v>180</v>
       </c>
-      <c r="G46" s="72"/>
-    </row>
-    <row r="47" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A47" s="70" t="s">
+      <c r="G46" s="56"/>
+    </row>
+    <row r="47" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="B47" s="71">
+      <c r="B47" s="55">
         <v>41</v>
       </c>
-      <c r="C47" s="71">
+      <c r="C47" s="55">
         <v>45</v>
       </c>
-      <c r="D47" s="68" t="s">
+      <c r="D47" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="E47" s="70" t="s">
+      <c r="E47" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="F47" s="70" t="s">
+      <c r="F47" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="G47" s="72"/>
-    </row>
-    <row r="48" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A48" s="70" t="s">
+      <c r="G47" s="56"/>
+    </row>
+    <row r="48" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="B48" s="70" t="s">
+      <c r="B48" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="71">
+      <c r="C48" s="55">
         <v>46</v>
       </c>
-      <c r="D48" s="68" t="s">
+      <c r="D48" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="70" t="s">
+      <c r="E48" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="F48" s="70" t="s">
+      <c r="F48" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="G48" s="69" t="s">
+      <c r="G48" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A49" s="70" t="s">
+    <row r="49" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="B49" s="70" t="s">
+      <c r="B49" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="71">
+      <c r="C49" s="55">
         <v>47</v>
       </c>
-      <c r="D49" s="68" t="s">
+      <c r="D49" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="E49" s="70" t="s">
+      <c r="E49" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="F49" s="70" t="s">
+      <c r="F49" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="G49" s="69" t="s">
+      <c r="G49" s="53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A50" s="70" t="s">
+    <row r="50" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="B50" s="71">
+      <c r="B50" s="55">
         <v>45</v>
       </c>
-      <c r="C50" s="71">
+      <c r="C50" s="55">
         <v>48</v>
       </c>
-      <c r="D50" s="68" t="s">
+      <c r="D50" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="E50" s="70" t="s">
+      <c r="E50" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="G50" s="72"/>
-    </row>
-    <row r="51" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A51" s="70" t="s">
+      <c r="G50" s="56"/>
+    </row>
+    <row r="51" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="B51" s="71">
+      <c r="B51" s="55">
         <v>45</v>
       </c>
-      <c r="C51" s="71">
+      <c r="C51" s="55">
         <v>49</v>
       </c>
-      <c r="D51" s="68" t="s">
+      <c r="D51" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="E51" s="70" t="s">
+      <c r="E51" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="F51" s="70" t="s">
+      <c r="F51" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="G51" s="72"/>
-    </row>
-    <row r="52" spans="1:7" ht="63.6" customHeight="1">
-      <c r="A52" s="70" t="s">
+      <c r="G51" s="56"/>
+    </row>
+    <row r="52" spans="1:7" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="B52" s="71">
+      <c r="B52" s="55">
         <v>45</v>
       </c>
-      <c r="C52" s="71">
+      <c r="C52" s="55">
         <v>50</v>
       </c>
-      <c r="D52" s="68" t="s">
+      <c r="D52" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="70" t="s">
+      <c r="E52" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="F52" s="70" t="s">
+      <c r="F52" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="G52" s="72"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="G53" s="76"/>
+      <c r="G52" s="56"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="G53" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4208,156 +4192,158 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="163.42578125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="167.28515625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="22" customWidth="1"/>
-    <col min="7" max="27" width="8.85546875" style="22" customWidth="1"/>
-    <col min="28" max="16384" width="8.85546875" style="22"/>
+    <col min="1" max="1" width="17.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="100.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="163.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="167.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="15" customWidth="1"/>
+    <col min="7" max="27" width="8.85546875" style="15" customWidth="1"/>
+    <col min="28" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="35.450000000000003" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:26" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="28"/>
-    </row>
-    <row r="2" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A2" s="29">
+      <c r="G1" s="73"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="17"/>
+    </row>
+    <row r="2" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="55">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="72">
+        <v>4</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="55">
+        <v>2</v>
+      </c>
+      <c r="B3" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="31">
-        <v>4</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="34"/>
-    </row>
-    <row r="3" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A3" s="35">
-        <v>2</v>
-      </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="72">
+        <v>10</v>
+      </c>
+      <c r="F3" s="70"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+    </row>
+    <row r="4" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="55">
+        <v>3</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="E3" s="17">
-        <v>10</v>
-      </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-    </row>
-    <row r="4" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A4" s="37">
-        <v>3</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="69" t="s">
         <v>211</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="21">
+      <c r="E4" s="72">
         <v>9</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="63"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -4378,24 +4364,24 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A5" s="37">
+    <row r="5" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="55">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="69" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="E5" s="72">
         <v>11</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -4416,24 +4402,24 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A6" s="37">
+    <row r="6" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="55">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="E6" s="21">
+      <c r="E6" s="72">
         <v>28</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="63"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -4454,24 +4440,24 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A7" s="37">
+    <row r="7" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="55">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7" s="21">
+      <c r="E7" s="72">
         <v>25</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="63"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -4492,24 +4478,24 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="50.45" customHeight="1">
-      <c r="A8" s="37">
+    <row r="8" spans="1:26" ht="50.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="55">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="69" t="s">
         <v>223</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E8" s="21">
+      <c r="E8" s="72">
         <v>24</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -4530,13 +4516,13 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="13.7" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+    <row r="9" spans="1:26" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -4558,9 +4544,9 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="13.7" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+    <row r="10" spans="1:26" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -4599,106 +4585,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.6" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="39" customWidth="1"/>
-    <col min="2" max="2" width="98.42578125" style="39" customWidth="1"/>
-    <col min="3" max="6" width="8.85546875" style="39" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="39"/>
+    <col min="1" max="1" width="4.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="98.42578125" style="21" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="66.95" customHeight="1">
-      <c r="A1" s="59" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="60"/>
+    <row r="1" spans="1:5" ht="66.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="42"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>228</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>229</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A3" s="42">
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A4" s="42">
+    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A5" s="42">
+    <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A6" s="42">
+    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="15.6" customHeight="1">
-      <c r="A7" s="42">
+    <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>234</v>
+      <c r="B7" s="25" t="s">
+        <v>233</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="13.7" customHeight="1">
-      <c r="A8" s="44"/>
+    <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" ht="13.7" customHeight="1">
+    <row r="9" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="13.7" customHeight="1">
+    <row r="10" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>

</xml_diff>